<commit_message>
changing placement of in door in room 101 because you come out stuck
</commit_message>
<xml_diff>
--- a/cube_mazes/10.xlsx
+++ b/cube_mazes/10.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23801"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24701"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Javascript_Misc\maze_messing_1\cube_mazes\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{028386B3-11CA-4EE8-8192-568D148CE38D}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5F70A244-4E1E-4EEE-A32D-A4D772E01C2A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="600" windowWidth="28800" windowHeight="15600" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="0" sheetId="1" r:id="rId1"/>
@@ -177,7 +177,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="34">
+  <fills count="35">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -363,6 +363,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="10">
     <border>
@@ -524,9 +530,10 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -896,7 +903,7 @@
   <dimension ref="A1:AI35"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="Q33" sqref="Q33"/>
+      <selection activeCell="AB26" sqref="AB26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3662,8 +3669,8 @@
       <c r="AA26" t="s">
         <v>0</v>
       </c>
-      <c r="AB26" t="s">
-        <v>1</v>
+      <c r="AB26" s="1" t="s">
+        <v>4</v>
       </c>
       <c r="AC26" t="s">
         <v>0</v>
@@ -3769,8 +3776,8 @@
       <c r="AA27" t="s">
         <v>0</v>
       </c>
-      <c r="AB27" s="1" t="s">
-        <v>4</v>
+      <c r="AB27" s="2" t="s">
+        <v>1</v>
       </c>
       <c r="AC27" t="s">
         <v>0</v>

</xml_diff>

<commit_message>
changing goal maze 23
</commit_message>
<xml_diff>
--- a/cube_mazes/10.xlsx
+++ b/cube_mazes/10.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Javascript_Misc\maze_messing_1\cube_mazes\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5F70A244-4E1E-4EEE-A32D-A4D772E01C2A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0C19EF0A-1537-4321-AB12-9DBE5B7A8D7B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="600" windowWidth="28800" windowHeight="15600" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -177,7 +177,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="35">
+  <fills count="34">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -363,12 +363,6 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="0"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
   </fills>
   <borders count="10">
     <border>
@@ -530,10 +524,9 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -903,7 +896,7 @@
   <dimension ref="A1:AI35"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="AB26" sqref="AB26"/>
+      <selection activeCell="AB27" sqref="AB27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3670,7 +3663,7 @@
         <v>0</v>
       </c>
       <c r="AB26" s="1" t="s">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="AC26" t="s">
         <v>0</v>
@@ -3776,8 +3769,8 @@
       <c r="AA27" t="s">
         <v>0</v>
       </c>
-      <c r="AB27" s="2" t="s">
-        <v>1</v>
+      <c r="AB27" s="1" t="s">
+        <v>4</v>
       </c>
       <c r="AC27" t="s">
         <v>0</v>

</xml_diff>